<commit_message>
transfer the project to a Class project make some changes in Excel file
</commit_message>
<xml_diff>
--- a/files/excel/weeding.xlsx
+++ b/files/excel/weeding.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ERAN LEVY\PycharmProjects\seatMe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ERAN LEVY\PycharmProjects\seatMe\files\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B3E6DE-43CD-4308-B39A-D233BAEFD846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C020691-3698-4E1D-85B3-635D890E27F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="##########"/>
+    <numFmt numFmtId="164" formatCode="##########"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -104,7 +104,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,7 +388,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="1">
-        <v>544743313</v>
+        <v>111111111</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -467,7 +467,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1">
-        <v>524350004</v>
+        <v>222222222</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="1">
-        <v>544792498</v>
+        <v>222222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the project and making the output message to be as a Label and not as messageinfo. Update also the pictures in readme
</commit_message>
<xml_diff>
--- a/files/excel/weeding.xlsx
+++ b/files/excel/weeding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ERAN LEVY\PycharmProjects\seatMe\files\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C020691-3698-4E1D-85B3-635D890E27F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B55C11-A218-4E1D-8E9F-033D5591BF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1">
-        <v>222222222</v>
+        <v>333333333</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>